<commit_message>
Main changes; made an R file for general simulation functions. Created a new simulation study DGP1 with Piecewise sinusoids and discontinuity.
</commit_message>
<xml_diff>
--- a/output/rf_waveform_output.xlsx
+++ b/output/rf_waveform_output.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\OneDrive\Bureaublad\msc_thesis\thesis_code\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5cac48941448979/Bureaublad/msc_thesis/thesis_code/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFC00BE-3469-4880-92AA-059E7B57974F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_42CED8001407EB9E70ECABD30CF720EDE9E2BF2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAC21893-8376-401B-BB3F-7031B9B08805}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>avg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">std </t>
   </si>
   <si>
     <t>std</t>
@@ -379,77 +376,77 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>0.186</v>
+        <v>0.184</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.19800000000000001</v>
+        <v>0.154</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.182</v>
+        <v>0.19400000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.17399999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.16400000000000001</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0.21199999999999999</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.22600000000000001</v>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0.152</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0.19800000000000001</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0.16200000000000001</v>
+        <v>0.17799999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="B12" t="s">
         <v>0</v>
       </c>
-      <c r="B12">
-        <f xml:space="preserve"> AVERAGE(A1:A10)</f>
-        <v>0.18539999999999998</v>
-      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13">
+        <f>_xlfn.STDEV.S(A1:A10)</f>
+        <v>2.1255064755906515E-2</v>
+      </c>
+      <c r="B13" t="s">
         <v>1</v>
-      </c>
-      <c r="B13">
-        <f>_xlfn.STDEV.S(A1:A10)</f>
-        <v>2.3419839642681069E-2</v>
       </c>
     </row>
   </sheetData>
@@ -463,77 +460,77 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>0.27972158400000002</v>
+        <v>0.27806748799999997</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.27670449600000002</v>
+        <v>0.26949211200000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.28944798399999999</v>
+        <v>0.29549150400000002</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.29500857600000002</v>
+        <v>0.25762707200000001</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.30464179200000002</v>
+        <v>0.27116889599999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0.30502649599999998</v>
+        <v>0.29406406400000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.33174118400000002</v>
+        <v>0.26478438399999998</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0.26600780800000001</v>
+        <v>0.30042103999999997</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0.28055708800000001</v>
+        <v>0.27671766399999997</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0.29129070400000001</v>
+        <v>0.28371555199999998</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>0.27915497760000002</v>
+      </c>
+      <c r="B12" t="s">
         <v>0</v>
       </c>
-      <c r="B12">
-        <f>AVERAGE(A1:A10)</f>
-        <v>0.29201477120000002</v>
-      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13">
+      <c r="A13">
         <f>_xlfn.STDEV.S(A1:A10)</f>
-        <v>1.860757810070035E-2</v>
+        <v>1.4128157397506419E-2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>